<commit_message>
new kw and excel modify
</commit_message>
<xml_diff>
--- a/regression-tests/src/test/java/com/hansencx/portal/testscripts/CancelBillingTests.xlsx
+++ b/regression-tests/src/test/java/com/hansencx/portal/testscripts/CancelBillingTests.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="14820" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="19380" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>Run mode</t>
   </si>
@@ -68,9 +68,6 @@
     <t>select count(KY_BA) from custpro.cpm_pnd_tran_hdr where ky_enroll in(select ky_enroll from custpro.cpm_pnd_tran_hdr where ky_pnd_seq_trans = 61761469)</t>
   </si>
   <si>
-    <t>output number of ky_ba</t>
-  </si>
-  <si>
     <t>check value</t>
   </si>
   <si>
@@ -78,12 +75,22 @@
   </si>
   <si>
     <t>output ky_ba</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>9041383009</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,17 +411,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="5" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -466,7 +473,7 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -477,14 +484,14 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="str">
         <f>I2</f>
-        <v>output number of ky_ba</v>
+        <v>out</v>
       </c>
       <c r="E3">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -498,10 +505,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -512,7 +519,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="str">
         <f>I4</f>

</xml_diff>

<commit_message>
commit excel keyword and some methods for page objects
</commit_message>
<xml_diff>
--- a/regression-tests/src/test/java/com/hansencx/portal/testscripts/CancelBillingTests.xlsx
+++ b/regression-tests/src/test/java/com/hansencx/portal/testscripts/CancelBillingTests.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="19380" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="20520" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Run mode</t>
   </si>
@@ -62,37 +62,47 @@
     <t>Y</t>
   </si>
   <si>
-    <t>execute query</t>
-  </si>
-  <si>
-    <t>select count(KY_BA) from custpro.cpm_pnd_tran_hdr where ky_enroll in(select ky_enroll from custpro.cpm_pnd_tran_hdr where ky_pnd_seq_trans = 61761469)</t>
-  </si>
-  <si>
-    <t>check value</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> select distinct KY_BA from custpro.cpm_pnd_tran_hdr where ky_enroll in(select ky_enroll from custpro.cpm_pnd_tran_hdr where ky_pnd_seq_trans = 61761469)</t>
-  </si>
-  <si>
-    <t>output ky_ba</t>
-  </si>
-  <si>
-    <t>out</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>9041383009</t>
+    <t>navigate to portal</t>
+  </si>
+  <si>
+    <t>log in to portal</t>
+  </si>
+  <si>
+    <t>QAGENERIC</t>
+  </si>
+  <si>
+    <t>QA!generic1</t>
+  </si>
+  <si>
+    <t>navigate to service center update secion</t>
+  </si>
+  <si>
+    <t>service update - click add new</t>
+  </si>
+  <si>
+    <t>service update add new - scroll to custpro aread</t>
+  </si>
+  <si>
+    <t>service update add new - select cancel rebill checkbox</t>
+  </si>
+  <si>
+    <t>service update add new - click import button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -128,7 +138,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,19 +419,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="5" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -469,12 +479,6 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -484,14 +488,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="str">
-        <f>I2</f>
-        <v>out</v>
-      </c>
-      <c r="E3">
-        <v>56</v>
+      <c r="E3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -502,13 +505,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -519,14 +516,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="str">
-        <f>I4</f>
-        <v>output ky_ba</v>
-      </c>
-      <c r="E5">
-        <v>9041383009</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -536,6 +526,9 @@
       <c r="B6">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -543,6 +536,20 @@
       </c>
       <c r="B7">
         <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>